<commit_message>
Another try at the schedule
</commit_message>
<xml_diff>
--- a/resources/ScheduleOfTopics.xlsx
+++ b/resources/ScheduleOfTopics.xlsx
@@ -555,7 +555,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E24" sqref="A1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -967,7 +967,7 @@
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
   <webPublishItems count="2">
     <webPublishItem id="30402" divId="ScheduleOfTopics_30402" sourceType="sheet" destinationFile="C:\aaaWork\Web\GitHub\NCMTH107\resources\ScheduleOfTopics.html" autoRepublish="1"/>
-    <webPublishItem id="25497" divId="ScheduleOfTopics_25497" sourceType="range" sourceRef="A1:E24" destinationFile="C:\aaaWork\Web\GitHub\NCMTH107\resources\ScheduleOfTopics.html" title="Tentative Schedule of Topics" autoRepublish="1"/>
+    <webPublishItem id="22338" divId="ScheduleOfTopics_22338" sourceType="sheet" destinationFile="C:\aaaWork\Web\GitHub\NCMTH107\resources\ScheduleOfTopics.html" autoRepublish="1"/>
   </webPublishItems>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
More updates to syllabus
</commit_message>
<xml_diff>
--- a/resources/ScheduleOfTopics.xlsx
+++ b/resources/ScheduleOfTopics.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -96,6 +97,15 @@
   </si>
   <si>
     <t>IVPPSS and Variable Types; Rstudio</t>
+  </si>
+  <si>
+    <t>Why Stats is important</t>
+  </si>
+  <si>
+    <t>Syllabus. Class Preparation</t>
+  </si>
+  <si>
+    <t>IVPPSS; Variable Types</t>
   </si>
 </sst>
 </file>
@@ -171,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,11 +232,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -265,8 +284,20 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,22 +579,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.25" customWidth="1"/>
-    <col min="4" max="4" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -578,385 +609,375 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="19.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
-        <v>41885</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>42382</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="12">
         <f>A24+3</f>
-        <v>41939</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42436</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="J2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13">
         <f>A2+2</f>
-        <v>41887</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>42384</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="13">
         <f>D2+2</f>
-        <v>41941</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42438</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <f>A3+3</f>
-        <v>41890</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>42387</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="13">
         <f>D3+2</f>
-        <v>41943</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42440</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <f>A4+2</f>
-        <v>41892</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>42389</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="13">
         <f>D4+3</f>
-        <v>41946</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42443</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <f>A5+2</f>
-        <v>41894</v>
+        <v>42391</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="13">
         <f>D5+2</f>
-        <v>41948</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42445</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="J6" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <f>A6+3</f>
-        <v>41897</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>42394</v>
+      </c>
+      <c r="B7" s="4"/>
       <c r="C7" s="1"/>
       <c r="D7" s="13">
         <f>D6+2</f>
-        <v>41950</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42447</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="J7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <f>A7+2</f>
-        <v>41899</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>42396</v>
+      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="1"/>
       <c r="D8" s="13">
         <f>D7+3</f>
-        <v>41953</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42450</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="J8" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <f>A8+2</f>
-        <v>41901</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>42398</v>
+      </c>
+      <c r="B9" s="4"/>
       <c r="C9" s="1"/>
       <c r="D9" s="13">
         <f>D8+2</f>
-        <v>41955</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42452</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <f>A9+3</f>
-        <v>41904</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
+        <v>42401</v>
+      </c>
+      <c r="B10" s="4"/>
       <c r="C10" s="1"/>
       <c r="D10" s="13">
         <f>D9+2</f>
-        <v>41957</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42454</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13">
         <f>A10+2</f>
-        <v>41906</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
-      </c>
+        <v>42403</v>
+      </c>
+      <c r="B11" s="5"/>
       <c r="C11" s="1"/>
       <c r="D11" s="13">
         <f>D10+3</f>
-        <v>41960</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42457</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="J11" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13">
         <f>A11+2</f>
-        <v>41908</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>42405</v>
+      </c>
+      <c r="B12" s="6"/>
       <c r="C12" s="1"/>
       <c r="D12" s="13">
         <f>D11+2</f>
-        <v>41962</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42459</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="J12" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13">
         <f>A12+3</f>
-        <v>41911</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>42408</v>
+      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="1"/>
       <c r="D13" s="13">
         <f>D12+2</f>
-        <v>41964</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42461</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="J13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13">
         <f>A13+2</f>
-        <v>41913</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>42410</v>
+      </c>
+      <c r="B14" s="5"/>
       <c r="C14" s="1"/>
       <c r="D14" s="13">
         <f>D13+3</f>
-        <v>41967</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42464</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <f>A14+2</f>
-        <v>41915</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>42412</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="13">
         <f>D14+2</f>
-        <v>41969</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42466</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="J15" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13">
         <f>A15+3</f>
-        <v>41918</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>42415</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="1"/>
       <c r="D16" s="13">
         <f>D15+2</f>
-        <v>41971</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42468</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <f>A16+2</f>
-        <v>41920</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>42417</v>
+      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="1"/>
       <c r="D17" s="13">
         <f>D16+3</f>
-        <v>41974</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42471</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="J17" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f>A17+2</f>
-        <v>41922</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>42419</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="13">
         <f>D17+2</f>
-        <v>41976</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42473</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f>A18+3</f>
-        <v>41925</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>42422</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="1"/>
       <c r="D19" s="13">
         <f>D18+2</f>
-        <v>41978</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42475</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f>A19+2</f>
-        <v>41927</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>42424</v>
+      </c>
+      <c r="B20" s="4"/>
       <c r="C20" s="1"/>
       <c r="D20" s="13">
         <f>D19+3</f>
-        <v>41981</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42478</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f>A20+2</f>
-        <v>41929</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>42426</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="1"/>
       <c r="D21" s="13">
         <f>D20+2</f>
-        <v>41983</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42480</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <f>A21+3</f>
-        <v>41932</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>17</v>
-      </c>
+        <v>42429</v>
+      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="1"/>
       <c r="D22" s="13">
         <f>D21+2</f>
-        <v>41985</v>
+        <v>42482</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <f>A22+2</f>
-        <v>41934</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>11</v>
-      </c>
+        <v>42431</v>
+      </c>
+      <c r="B23" s="6"/>
       <c r="C23" s="1"/>
       <c r="D23" s="14"/>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <f>A23+2</f>
-        <v>41936</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>12</v>
-      </c>
+        <v>42433</v>
+      </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -965,4 +986,199 @@
     <webPublishItem id="25497" divId="ScheduleOfTopics_25497" sourceType="range" sourceRef="A1:E24" destinationFile="C:\aaaWork\Web\GitHub\NCMTH107\resources\ScheduleOfTopics.html"/>
   </webPublishItems>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more to NormDist CEs
</commit_message>
<xml_diff>
--- a/resources/ScheduleOfTopics.xlsx
+++ b/resources/ScheduleOfTopics.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -594,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -623,6 +623,9 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" spans="1:10" ht="19.7" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
@@ -638,7 +641,7 @@
       </c>
       <c r="E2" s="3"/>
       <c r="J2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -658,7 +661,7 @@
         <v>17</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -678,7 +681,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -696,7 +699,7 @@
       </c>
       <c r="E5" s="4"/>
       <c r="J5" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -714,7 +717,7 @@
       </c>
       <c r="E6" s="4"/>
       <c r="J6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -732,7 +735,7 @@
       </c>
       <c r="E7" s="4"/>
       <c r="J7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -749,8 +752,8 @@
         <v>42450</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="J8" s="4" t="s">
-        <v>10</v>
+      <c r="J8" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -769,8 +772,8 @@
       <c r="E9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>22</v>
+      <c r="J9" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -789,8 +792,8 @@
       <c r="E10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>11</v>
+      <c r="J10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -807,8 +810,8 @@
         <v>42457</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="J11" s="7" t="s">
-        <v>12</v>
+      <c r="J11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -825,8 +828,8 @@
         <v>42459</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="J12" s="5" t="s">
-        <v>13</v>
+      <c r="J12" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -844,7 +847,7 @@
       </c>
       <c r="E13" s="4"/>
       <c r="J13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -861,8 +864,8 @@
         <v>42464</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="J14" s="4" t="s">
-        <v>16</v>
+      <c r="J14" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -879,8 +882,8 @@
         <v>42466</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="J15" s="4" t="s">
-        <v>16</v>
+      <c r="J15" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,20 +891,27 @@
         <f>A15+3</f>
         <v>42415</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="13">
         <f>D15+2</f>
         <v>42468</v>
       </c>
       <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13">
         <f>A16+2</f>
         <v>42417</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="13">
         <f>D16+3</f>
@@ -909,10 +919,10 @@
       </c>
       <c r="E17" s="6"/>
       <c r="J17" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13">
         <f>A17+2</f>
         <v>42419</v>
@@ -927,31 +937,32 @@
       </c>
       <c r="E18" s="4"/>
       <c r="J18" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13">
         <f>A18+3</f>
         <v>42422</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="13">
         <f>D18+2</f>
         <v>42475</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="J19" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13">
         <f>A19+2</f>
         <v>42424</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="13">
         <f>D19+3</f>
@@ -959,12 +970,14 @@
       </c>
       <c r="E20" s="6"/>
     </row>
-    <row r="21" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <f>A20+2</f>
         <v>42426</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C21" s="1"/>
       <c r="D21" s="13">
         <f>D20+2</f>
@@ -972,12 +985,14 @@
       </c>
       <c r="E21" s="6"/>
     </row>
-    <row r="22" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <f>A21+3</f>
         <v>42429</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="13">
         <f>D21+2</f>
@@ -986,11 +1001,8 @@
       <c r="E22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="L22" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <f>A22+2</f>
         <v>42431</v>
@@ -1000,7 +1012,7 @@
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:12" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="19.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <f>A23+2</f>
         <v>42433</v>
@@ -1024,7 +1036,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A20"/>
+      <selection activeCell="F1" sqref="F1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>